<commit_message>
changed R value from 30k to 33k
changed r value to lower supply current.
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for Heliotrope_Logic_v2/BOM/Bill of Materials-Heliotrope_Logic_v2.xlsx
+++ b/Hardware/Project Outputs for Heliotrope_Logic_v2/BOM/Bill of Materials-Heliotrope_Logic_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Heliotrope_Logic_v2\Project Outputs for Heliotrope_Logic_v2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27579432-395B-48BC-86A1-2CFD70481FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{98565502-BB46-4541-A38D-DDBE4789D07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="4470" windowWidth="18720" windowHeight="15435" xr2:uid="{4E26B8CF-CF38-4E24-B085-824823E0080D}"/>
+    <workbookView xWindow="14205" yWindow="4470" windowWidth="18720" windowHeight="15435" xr2:uid="{8FF9D92E-0A1A-42D0-B99A-8659DB0B8672}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Heliotrope_Lo" sheetId="1" r:id="rId1"/>
@@ -236,10 +236,10 @@
     <t>R4</t>
   </si>
   <si>
-    <t>RMCF0603FT30K0</t>
-  </si>
-  <si>
-    <t>Res Thick Film 0603 30K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD Automotive T/R</t>
+    <t>RMCF0603FT33K0</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0603 33K Ohm 1% 0.1W(1/10W) ±100ppm/C Pad SMD Automotive T/R</t>
   </si>
   <si>
     <t>R2</t>
@@ -657,7 +657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4703323-8D77-4040-A5A3-04BD7DF2B8D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AC5275-F43C-4660-8840-C90293900027}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
fixed another R value and math
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for Heliotrope_Logic_v2/BOM/Bill of Materials-Heliotrope_Logic_v2.xlsx
+++ b/Hardware/Project Outputs for Heliotrope_Logic_v2/BOM/Bill of Materials-Heliotrope_Logic_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Heliotrope_Logic_v2\Project Outputs for Heliotrope_Logic_v2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98565502-BB46-4541-A38D-DDBE4789D07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84D24035-E228-4D1D-B794-65364E1272E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="4470" windowWidth="18720" windowHeight="15435" xr2:uid="{8FF9D92E-0A1A-42D0-B99A-8659DB0B8672}"/>
+    <workbookView xWindow="14205" yWindow="4470" windowWidth="18720" windowHeight="15435" xr2:uid="{CFC77EDB-E49C-4A7C-9D07-4ED50826BCFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Heliotrope_Lo" sheetId="1" r:id="rId1"/>
@@ -657,7 +657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76AC5275-F43C-4660-8840-C90293900027}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96028CDD-9F56-4A8A-9358-3A42F2D02887}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
changed power trace from 10mill to 20mill
</commit_message>
<xml_diff>
--- a/Hardware/Project Outputs for Heliotrope_Logic_v2/BOM/Bill of Materials-Heliotrope_Logic_v2.xlsx
+++ b/Hardware/Project Outputs for Heliotrope_Logic_v2/BOM/Bill of Materials-Heliotrope_Logic_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Heliotrope_Logic_v2\Project Outputs for Heliotrope_Logic_v2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CE8FFE4-23C7-4CDF-90B4-F905D34DAF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4E3D960-98CA-4941-94A7-E7549DF779A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="4470" windowWidth="18720" windowHeight="15435" xr2:uid="{5EB8D918-291D-4C86-B133-D1367FECDF95}"/>
+    <workbookView xWindow="13500" yWindow="3495" windowWidth="18720" windowHeight="15435" xr2:uid="{566F9ADB-E820-40BB-AB03-8365BB19BFB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Heliotrope_Lo" sheetId="1" r:id="rId1"/>
@@ -657,7 +657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F696A0CB-0D5C-4A44-A4BA-885B58627D3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B59A95A-0284-476C-A79C-B243FEC9EB5F}">
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>